<commit_message>
solver example updated & working
</commit_message>
<xml_diff>
--- a/linear_programming/Modeling/Madona/LPM-madona.xlsx
+++ b/linear_programming/Modeling/Madona/LPM-madona.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1517766115.CIV\Desktop\Modeling\Madona\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmc/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="420" windowWidth="20475" windowHeight="12000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sensitivity Report 1" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,12 @@
     <sheet name="myVersion" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">myVersion!$J$11:$L$21,myVersion!$J$11:$L$21</definedName>
+    <definedName name="AmtPaidConstraint">myVersion!$E$11:$E$22</definedName>
+    <definedName name="InterestConstraint">myVersion!$Q$11:$S$22</definedName>
+    <definedName name="Lij">myVersion!$J$11:$L$22</definedName>
+    <definedName name="NoDebtConstraint">myVersion!$J$22:$L$22</definedName>
+    <definedName name="Objective">myVersion!$H$3</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">myVersion!$B$11:$D$22,myVersion!$J$11:$L$22</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet1!$B$4:$D$16,Sheet1!$F$4:$H$16</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
@@ -29,15 +34,18 @@
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs0" localSheetId="2" hidden="1">myVersion!$E$10:$E$21</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">myVersion!$B$10:$D$21</definedName>
+    <definedName name="solver_lhs0" localSheetId="2" hidden="1">myVersion!$E$11:$E$22</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">myVersion!$Q$11:$S$22</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet1!$E$16:$H$16</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">myVersion!$E$10:$E$21</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">myVersion!$E$11:$E$22</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet1!$E$4:$E$16</definedName>
-    <definedName name="solver_lhs3" localSheetId="2" hidden="1">myVersion!$J$10:$L$21</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">myVersion!$J$11:$L$22</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">Sheet1!$I$4:$K$16</definedName>
-    <definedName name="solver_lhs4" localSheetId="2" hidden="1">myVersion!$J$21:$L$21</definedName>
-    <definedName name="solver_lhs5" localSheetId="2" hidden="1">myVersion!$Q$11:$S$21</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">myVersion!$J$22:$L$22</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">myVersion!$B$11:$D$22</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">myVersion!$B$11:$D$22</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
@@ -61,15 +69,16 @@
     <definedName name="solver_rbv" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel0" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel5" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rhs0" localSheetId="2" hidden="1">myVersion!$G$10:$G$21</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rhs0" localSheetId="2" hidden="1">myVersion!$G$11:$G$22</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">10000</definedName>
@@ -78,6 +87,7 @@
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
@@ -96,12 +106,19 @@
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="Xij">myVersion!$B$11:$D$22</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -109,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>foot</t>
   </si>
@@ -268,6 +285,30 @@
   </si>
   <si>
     <t>Obj.</t>
+  </si>
+  <si>
+    <t>Total Debt</t>
+  </si>
+  <si>
+    <t>Total Debt + Interest</t>
+  </si>
+  <si>
+    <t>Extra Paid / Month</t>
+  </si>
+  <si>
+    <t>Posterior Analysis</t>
+  </si>
+  <si>
+    <t>Credit Card Look Up Table</t>
+  </si>
+  <si>
+    <t>Xij</t>
+  </si>
+  <si>
+    <t>Lij</t>
+  </si>
+  <si>
+    <t>Interst Constraint!</t>
   </si>
 </sst>
 </file>
@@ -331,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -379,56 +420,56 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color theme="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color theme="1"/>
@@ -438,39 +479,48 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color theme="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -507,12 +557,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -531,10 +575,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -600,9 +653,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -635,9 +688,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -821,38 +874,38 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
@@ -871,7 +924,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
@@ -894,7 +947,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
@@ -917,7 +970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -940,12 +993,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
@@ -964,7 +1017,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
@@ -987,7 +1040,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -1010,7 +1063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1033,7 +1086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1065,33 +1118,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="F1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>30</v>
       </c>
@@ -1126,7 +1179,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>0</v>
       </c>
@@ -1147,7 +1200,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1186,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1221,11 +1274,11 @@
         <v>0</v>
       </c>
       <c r="K5" s="8">
-        <f t="shared" ref="K5:K39" si="3">H4*(1+0.015)-D5-H5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <f>H4*(1+0.015)-D5-H5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1260,11 +1313,11 @@
         <v>0</v>
       </c>
       <c r="K6" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" ref="K6:K39" si="3">H5*(1+0.015)-D6-H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1303,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1342,7 +1395,7 @@
         <v>-1.5916157281026244E-12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1381,7 +1434,7 @@
         <v>-6.0163074522279205E-12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -1420,7 +1473,7 @@
         <v>1.4539409676217472E-11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -1459,7 +1512,7 @@
         <v>-1.3187673175707459E-11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -1498,7 +1551,7 @@
         <v>7.7011463872622693E-12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1537,7 +1590,7 @@
         <v>-4.5474735088646412E-13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -1576,7 +1629,7 @@
         <v>-1.8189894035458565E-12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -1615,7 +1668,7 @@
         <v>9.0949470177292824E-13</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -1654,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -1696,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -1735,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -1774,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -1813,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -1852,7 +1905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>19</v>
       </c>
@@ -1885,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -1918,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>21</v>
       </c>
@@ -1951,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -1984,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>23</v>
       </c>
@@ -2017,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>24</v>
       </c>
@@ -2050,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>25</v>
       </c>
@@ -2083,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>26</v>
       </c>
@@ -2116,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>27</v>
       </c>
@@ -2149,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>28</v>
       </c>
@@ -2182,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>29</v>
       </c>
@@ -2215,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>30</v>
       </c>
@@ -2248,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>31</v>
       </c>
@@ -2281,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>32</v>
       </c>
@@ -2314,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>33</v>
       </c>
@@ -2347,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>34</v>
       </c>
@@ -2380,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>35</v>
       </c>
@@ -2413,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>36</v>
       </c>
@@ -2446,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B40" s="6">
         <f>SUM(B4:B39)</f>
         <v>21137.036884629622</v>
@@ -2460,7 +2513,7 @@
         <v>41568.690899124987</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>38</v>
       </c>
@@ -2481,55 +2534,95 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:U21"/>
+  <dimension ref="A2:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G21"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="J2" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+    </row>
+    <row r="3" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="13" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>52</v>
       </c>
       <c r="H3" s="6">
-        <f>SUM(B10:D21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+        <f>SUM(B11:D22)</f>
+        <v>115581.7046707625</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="14">
         <v>20000</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>50000</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>40000</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="J4" s="6">
+        <f>SUM(C4:E4)</f>
+        <v>110000</v>
+      </c>
+      <c r="K4" s="20">
+        <f>Objective</f>
+        <v>115581.7046707625</v>
+      </c>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20">
+        <f>(K4-J4)/12</f>
+        <v>465.14205589687481</v>
+      </c>
+      <c r="N4" s="20"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="15">
         <v>1E-3</v>
       </c>
       <c r="D5" s="7">
@@ -2539,592 +2632,751 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="I8" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8"/>
+      <c r="B8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13">
-        <f>SUM(B10:D10)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J10" s="6">
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="P9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+    </row>
+    <row r="10" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7">
         <f>C$4</f>
         <v>20000</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="7">
         <f>D$4</f>
         <v>50000</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="7">
         <f>E$4</f>
         <v>40000</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="R10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="S10" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+    <row r="11" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E11" s="18">
+        <f>SUM(B11:D11)</f>
+        <v>10000</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8">
+        <v>20020</v>
+      </c>
+      <c r="K11" s="8">
+        <v>50500</v>
+      </c>
+      <c r="L11" s="8">
+        <v>30600.000000000004</v>
+      </c>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7">
+        <f>J10-(B11-J10*C$5)-J11</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="7">
+        <f>K10-(C11-K10*D$5)-K11</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="7">
+        <f>L10-(D11-L10*E$5)-L11</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="U11" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
         <v>2</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13">
-        <f t="shared" ref="E11:E21" si="0">SUM(B11:D11)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E12" s="18">
+        <f t="shared" ref="E12:E22" si="0">SUM(B12:D12)</f>
+        <v>10000</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J11" s="12">
-        <v>0</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0</v>
-      </c>
-      <c r="L11" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="6">
-        <f>J11-(B12+J11*C$5)-J12</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="6">
-        <f t="shared" ref="R11:S11" si="1">K11-(C12+K11*D$5)-K12</f>
-        <v>0</v>
-      </c>
-      <c r="S11" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T11" s="13" t="s">
+      <c r="G12" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8">
+        <v>20040.019999999997</v>
+      </c>
+      <c r="K12" s="8">
+        <v>51005.000000000015</v>
+      </c>
+      <c r="L12" s="8">
+        <v>21059.000000000011</v>
+      </c>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7">
+        <f>J11-(B12-J11*C$5)-J12</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="7">
+        <f>K11-(C12-K11*D$5)-K12</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="7">
+        <f>L11-(D12-L11*E$5)-L12</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U11" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="U12" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
         <v>3</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="13" t="s">
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E13" s="18">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J12" s="12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="6">
-        <f t="shared" ref="Q12:Q21" si="2">J12-(B13+J12*C$5)-J13</f>
-        <v>0</v>
-      </c>
-      <c r="R12" s="6">
-        <f t="shared" ref="R12:R21" si="3">K12-(C13+K12*D$5)-K13</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="6">
-        <f t="shared" ref="S12:S21" si="4">L12-(D13+L12*E$5)-L13</f>
-        <v>0</v>
-      </c>
-      <c r="T12" s="13" t="s">
+      <c r="G13" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="8">
+        <v>20060.060019999997</v>
+      </c>
+      <c r="K13" s="8">
+        <v>51515.05</v>
+      </c>
+      <c r="L13" s="8">
+        <v>11374.885000000006</v>
+      </c>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7">
+        <f>J12-(B13-J12*C$5)-J13</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="7">
+        <f>K12-(C13-K12*D$5)-K13</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="7">
+        <f>L12-(D13-L12*E$5)-L13</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U12" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="U13" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
         <v>4</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E14" s="18">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J13" s="12">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
-        <v>0</v>
-      </c>
-      <c r="L13" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="13" t="s">
+      <c r="G14" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8">
+        <v>20080.120080019991</v>
+      </c>
+      <c r="K14" s="8">
+        <v>52030.200500000006</v>
+      </c>
+      <c r="L14" s="8">
+        <v>1545.5082750000101</v>
+      </c>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7">
+        <f>J13-(B14-J13*C$5)-J14</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="7">
+        <f>K13-(C14-K13*D$5)-K14</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="7">
+        <f>L13-(D14-L13*E$5)-L14</f>
+        <v>-4.5474735088646412E-12</v>
+      </c>
+      <c r="T14" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U13" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="U14" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
         <v>5</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="13" t="s">
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>8431.3091008749961</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1568.6908991250039</v>
+      </c>
+      <c r="E15" s="18">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J14" s="12">
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <v>0</v>
-      </c>
-      <c r="L14" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S14" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="13" t="s">
+      <c r="G15" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="8">
+        <v>20100.200200100007</v>
+      </c>
+      <c r="K15" s="8">
+        <v>44119.193404124999</v>
+      </c>
+      <c r="L15" s="8">
+        <v>9.0949470177292824E-13</v>
+      </c>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7">
+        <f>J14-(B15-J14*C$5)-J15</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="7">
+        <f>K14-(C15-K14*D$5)-K15</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="7">
+        <f>L14-(D15-L14*E$5)-L15</f>
+        <v>5.4569682106375694E-12</v>
+      </c>
+      <c r="T15" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U14" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="U15" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
         <v>6</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="13" t="s">
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>10000</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="18">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J15" s="12">
-        <v>0</v>
-      </c>
-      <c r="K15" s="12">
-        <v>0</v>
-      </c>
-      <c r="L15" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S15" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T15" s="13" t="s">
+      <c r="G16" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8">
+        <v>20120.300400300104</v>
+      </c>
+      <c r="K16" s="8">
+        <v>34560.385338166256</v>
+      </c>
+      <c r="L16" s="8">
+        <v>1.8189894035458565E-12</v>
+      </c>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7">
+        <f>J15-(B16-J15*C$5)-J16</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="7">
+        <f>K15-(C16-K15*D$5)-K16</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="7">
+        <f>L15-(D16-L15*E$5)-L16</f>
+        <v>-8.958522812463344E-13</v>
+      </c>
+      <c r="T16" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U15" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="U16" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
         <v>7</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="13" t="s">
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>10000</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="18">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J16" s="12">
-        <v>0</v>
-      </c>
-      <c r="K16" s="12">
-        <v>0</v>
-      </c>
-      <c r="L16" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S16" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T16" s="13" t="s">
+      <c r="G17" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="8">
+        <v>20140.420700700404</v>
+      </c>
+      <c r="K17" s="8">
+        <v>24905.98919154792</v>
+      </c>
+      <c r="L17" s="8">
+        <v>1.3642420526593924E-12</v>
+      </c>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7">
+        <f>J16-(B17-J16*C$5)-J17</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="7">
+        <f>K16-(C17-K16*D$5)-K17</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="7">
+        <f>L16-(D17-L16*E$5)-L17</f>
+        <v>4.8203219193965179E-13</v>
+      </c>
+      <c r="T17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U16" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="U17" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
         <v>8</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="13" t="s">
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8">
+        <v>10000</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="18">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J17" s="12">
-        <v>0</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S17" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T17" s="13" t="s">
+      <c r="G18" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="8">
+        <v>20160.561121401101</v>
+      </c>
+      <c r="K18" s="8">
+        <v>15155.049083463404</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0</v>
+      </c>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7">
+        <f>J17-(B18-J17*C$5)-J18</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="7">
+        <f>K17-(C18-K17*D$5)-K18</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="7">
+        <f>L17-(D18-L17*E$5)-L18</f>
+        <v>1.3847056834492832E-12</v>
+      </c>
+      <c r="T18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U17" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="U18" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
         <v>9</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="13" t="s">
+      <c r="B19" s="8">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8">
+        <v>9999.9999999999982</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1.1368683772161603E-12</v>
+      </c>
+      <c r="E19" s="18">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J18" s="12">
-        <v>0</v>
-      </c>
-      <c r="K18" s="12">
-        <v>0</v>
-      </c>
-      <c r="L18" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S18" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T18" s="13" t="s">
+      <c r="G19" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="8">
+        <v>20180.721682522497</v>
+      </c>
+      <c r="K19" s="8">
+        <v>5306.5995742980385</v>
+      </c>
+      <c r="L19" s="8">
+        <v>3.1832314562052488E-12</v>
+      </c>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7">
+        <f>J18-(B19-J18*C$5)-J19</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="7">
+        <f>K18-(C19-K18*D$5)-K19</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="7">
+        <f>L18-(D19-L18*E$5)-L19</f>
+        <v>-4.3200998334214091E-12</v>
+      </c>
+      <c r="T19" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U18" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="U19" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
         <v>10</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="13" t="s">
+      <c r="B20" s="8">
+        <v>4640.3344299589871</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5359.6655700410165</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="18">
+        <f t="shared" si="0"/>
+        <v>10000.000000000004</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J19" s="12">
-        <v>0</v>
-      </c>
-      <c r="K19" s="12">
-        <v>0</v>
-      </c>
-      <c r="L19" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S19" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="13" t="s">
+      <c r="G20" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="8">
+        <v>15560.567974246031</v>
+      </c>
+      <c r="K20" s="8">
+        <v>0</v>
+      </c>
+      <c r="L20" s="8">
+        <v>0</v>
+      </c>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7">
+        <f>J19-(B20-J19*C$5)-J20</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="7">
+        <f>K19-(C20-K19*D$5)-K20</f>
+        <v>2.7284841053187847E-12</v>
+      </c>
+      <c r="S20" s="7">
+        <f>L19-(D20-L19*E$5)-L20</f>
+        <v>3.2309799280483278E-12</v>
+      </c>
+      <c r="T20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U19" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="U20" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
         <v>11</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="13" t="s">
+      <c r="B21" s="8">
+        <v>10000</v>
+      </c>
+      <c r="C21" s="8">
+        <v>9.0949470177292824E-13</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1.8189894035458565E-12</v>
+      </c>
+      <c r="E21" s="18">
+        <f t="shared" si="0"/>
+        <v>10000.000000000002</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J20" s="12">
-        <v>0</v>
-      </c>
-      <c r="K20" s="12">
-        <v>0</v>
-      </c>
-      <c r="L20" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S20" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="13" t="s">
+      <c r="G21" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8">
+        <v>5576.12854222028</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0</v>
+      </c>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7">
+        <f>J20-(B21-J20*C$5)-J21</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="7">
+        <f>K20-(C21-K20*D$5)-K21</f>
+        <v>-9.0949470177292824E-13</v>
+      </c>
+      <c r="S21" s="7">
+        <f>L20-(D21-L20*E$5)-L21</f>
+        <v>-1.8189894035458565E-12</v>
+      </c>
+      <c r="T21" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U20" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="U21" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
         <v>12</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="13" t="s">
+      <c r="B22" s="8">
+        <v>5581.704670762495</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="18">
+        <f t="shared" si="0"/>
+        <v>5581.704670762495</v>
+      </c>
+      <c r="F22" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="13">
-        <v>10000</v>
-      </c>
-      <c r="J21" s="12">
-        <v>0</v>
-      </c>
-      <c r="K21" s="12">
-        <v>0</v>
-      </c>
-      <c r="L21" s="12">
-        <v>0</v>
-      </c>
-      <c r="M21" s="13" t="s">
+      <c r="G22" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="8">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0</v>
+      </c>
+      <c r="L22" s="8">
+        <v>0</v>
+      </c>
+      <c r="M22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N21" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S21" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T21" s="13" t="s">
+      <c r="N22" s="18">
+        <v>0</v>
+      </c>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7">
+        <f>J21-(B22-J21*C$5)-J22</f>
+        <v>5.4569682106375694E-12</v>
+      </c>
+      <c r="R22" s="7">
+        <f>K21-(C22-K21*D$5)-K22</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="7">
+        <f>L21-(D22-L21*E$5)-L22</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="U21" s="13">
+      <c r="U22" s="18">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="9">
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B2:E2"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="I8:K8"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>